<commit_message>
Added required/restricted planet tag logic
</commit_message>
<xml_diff>
--- a/vfBattleTechMod-ProcGenStores-Test/res/test-xlrp-store-content.xlsx
+++ b/vfBattleTechMod-ProcGenStores-Test/res/test-xlrp-store-content.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Games\Steam\steamapps\common\BATTLETECH\Repository\vfBattleTechMod-Core\vfBattleTechMod-ProcGenStores-Test\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{685AF893-90BE-43A0-BDED-650CA6E6B036}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53FB639C-57C0-43C9-92EC-32BA21B23794}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="1830" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="1830" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Reference" sheetId="6" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4857" uniqueCount="609">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5249" uniqueCount="610">
   <si>
     <t>ActuatorTemplate</t>
   </si>
@@ -1851,7 +1851,10 @@
     <t>Restricted PlanetTags (Any of)</t>
   </si>
   <si>
-    <t>Very Uncommon</t>
+    <t>planet_test_MVP</t>
+  </si>
+  <si>
+    <t>planet_test_vengefire|planet_test_zappo</t>
   </si>
 </sst>
 </file>
@@ -2563,7 +2566,7 @@
   <dimension ref="A1:J135"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2628,6 +2631,12 @@
       <c r="G2" s="2" t="s">
         <v>473</v>
       </c>
+      <c r="I2" t="s">
+        <v>473</v>
+      </c>
+      <c r="J2" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
@@ -2651,6 +2660,12 @@
       <c r="G3" s="2" t="s">
         <v>473</v>
       </c>
+      <c r="I3" t="s">
+        <v>473</v>
+      </c>
+      <c r="J3" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
@@ -2674,6 +2689,12 @@
       <c r="G4" s="2" t="s">
         <v>476</v>
       </c>
+      <c r="I4" t="s">
+        <v>473</v>
+      </c>
+      <c r="J4" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
@@ -2697,6 +2718,12 @@
       <c r="G5" s="2" t="s">
         <v>476</v>
       </c>
+      <c r="I5" t="s">
+        <v>473</v>
+      </c>
+      <c r="J5" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
@@ -2720,6 +2747,12 @@
       <c r="G6" s="2" t="s">
         <v>476</v>
       </c>
+      <c r="I6" t="s">
+        <v>473</v>
+      </c>
+      <c r="J6" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
@@ -2743,6 +2776,12 @@
       <c r="G7" s="2" t="s">
         <v>476</v>
       </c>
+      <c r="I7" t="s">
+        <v>473</v>
+      </c>
+      <c r="J7" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
@@ -2766,6 +2805,12 @@
       <c r="G8" s="2" t="s">
         <v>476</v>
       </c>
+      <c r="I8" t="s">
+        <v>473</v>
+      </c>
+      <c r="J8" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
@@ -2789,6 +2834,12 @@
       <c r="G9" s="2" t="s">
         <v>476</v>
       </c>
+      <c r="I9" t="s">
+        <v>473</v>
+      </c>
+      <c r="J9" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
@@ -2812,6 +2863,12 @@
       <c r="G10" s="2" t="s">
         <v>476</v>
       </c>
+      <c r="I10" t="s">
+        <v>473</v>
+      </c>
+      <c r="J10" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
@@ -2835,6 +2892,12 @@
       <c r="G11" s="2" t="s">
         <v>473</v>
       </c>
+      <c r="I11" t="s">
+        <v>473</v>
+      </c>
+      <c r="J11" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
@@ -2858,6 +2921,12 @@
       <c r="G12" s="2" t="s">
         <v>482</v>
       </c>
+      <c r="I12" t="s">
+        <v>473</v>
+      </c>
+      <c r="J12" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
@@ -2881,6 +2950,12 @@
       <c r="G13" s="2" t="s">
         <v>473</v>
       </c>
+      <c r="I13" t="s">
+        <v>473</v>
+      </c>
+      <c r="J13" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
@@ -2904,6 +2979,12 @@
       <c r="G14" s="2" t="s">
         <v>475</v>
       </c>
+      <c r="I14" t="s">
+        <v>473</v>
+      </c>
+      <c r="J14" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
@@ -2927,6 +3008,12 @@
       <c r="G15" s="2" t="s">
         <v>473</v>
       </c>
+      <c r="I15" t="s">
+        <v>473</v>
+      </c>
+      <c r="J15" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
@@ -2950,8 +3037,14 @@
       <c r="G16" s="2" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="I16" t="s">
+        <v>473</v>
+      </c>
+      <c r="J16" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -2973,8 +3066,14 @@
       <c r="G17" s="2" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="I17" t="s">
+        <v>473</v>
+      </c>
+      <c r="J17" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -2996,8 +3095,14 @@
       <c r="G18" s="2" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="I18" t="s">
+        <v>473</v>
+      </c>
+      <c r="J18" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -3019,8 +3124,14 @@
       <c r="G19" s="2" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="20" spans="1:7">
+      <c r="I19" t="s">
+        <v>473</v>
+      </c>
+      <c r="J19" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -3042,8 +3153,14 @@
       <c r="G20" s="2" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="I20" t="s">
+        <v>473</v>
+      </c>
+      <c r="J20" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -3065,8 +3182,14 @@
       <c r="G21" s="2" t="s">
         <v>473</v>
       </c>
-    </row>
-    <row r="22" spans="1:7">
+      <c r="I21" t="s">
+        <v>473</v>
+      </c>
+      <c r="J21" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -3088,8 +3211,14 @@
       <c r="G22" s="2" t="s">
         <v>473</v>
       </c>
-    </row>
-    <row r="23" spans="1:7">
+      <c r="I22" t="s">
+        <v>473</v>
+      </c>
+      <c r="J22" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -3111,8 +3240,14 @@
       <c r="G23" s="2" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="24" spans="1:7">
+      <c r="I23" t="s">
+        <v>473</v>
+      </c>
+      <c r="J23" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -3134,8 +3269,14 @@
       <c r="G24" s="2" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="25" spans="1:7">
+      <c r="I24" t="s">
+        <v>473</v>
+      </c>
+      <c r="J24" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -3157,8 +3298,14 @@
       <c r="G25" s="2" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="26" spans="1:7">
+      <c r="I25" t="s">
+        <v>473</v>
+      </c>
+      <c r="J25" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -3180,8 +3327,14 @@
       <c r="G26" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="27" spans="1:7">
+      <c r="I26" t="s">
+        <v>473</v>
+      </c>
+      <c r="J26" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -3203,8 +3356,14 @@
       <c r="G27" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="28" spans="1:7">
+      <c r="I27" t="s">
+        <v>473</v>
+      </c>
+      <c r="J27" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -3226,8 +3385,14 @@
       <c r="G28" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="29" spans="1:7">
+      <c r="I28" t="s">
+        <v>473</v>
+      </c>
+      <c r="J28" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -3249,8 +3414,14 @@
       <c r="G29" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="30" spans="1:7">
+      <c r="I29" t="s">
+        <v>473</v>
+      </c>
+      <c r="J29" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -3272,8 +3443,14 @@
       <c r="G30" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="31" spans="1:7">
+      <c r="I30" t="s">
+        <v>473</v>
+      </c>
+      <c r="J30" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -3295,8 +3472,14 @@
       <c r="G31" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="32" spans="1:7">
+      <c r="I31" t="s">
+        <v>473</v>
+      </c>
+      <c r="J31" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -3318,8 +3501,14 @@
       <c r="G32" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="33" spans="1:7">
+      <c r="I32" t="s">
+        <v>473</v>
+      </c>
+      <c r="J32" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -3341,8 +3530,14 @@
       <c r="G33" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="34" spans="1:7">
+      <c r="I33" t="s">
+        <v>473</v>
+      </c>
+      <c r="J33" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -3364,8 +3559,14 @@
       <c r="G34" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="35" spans="1:7">
+      <c r="I34" t="s">
+        <v>473</v>
+      </c>
+      <c r="J34" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -3387,8 +3588,14 @@
       <c r="G35" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="36" spans="1:7">
+      <c r="I35" t="s">
+        <v>473</v>
+      </c>
+      <c r="J35" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -3410,8 +3617,14 @@
       <c r="G36" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="37" spans="1:7">
+      <c r="I36" t="s">
+        <v>473</v>
+      </c>
+      <c r="J36" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -3433,8 +3646,14 @@
       <c r="G37" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="38" spans="1:7">
+      <c r="I37" t="s">
+        <v>473</v>
+      </c>
+      <c r="J37" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -3456,8 +3675,14 @@
       <c r="G38" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="39" spans="1:7">
+      <c r="I38" t="s">
+        <v>473</v>
+      </c>
+      <c r="J38" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -3479,8 +3704,14 @@
       <c r="G39" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="40" spans="1:7">
+      <c r="I39" t="s">
+        <v>473</v>
+      </c>
+      <c r="J39" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -3502,8 +3733,14 @@
       <c r="G40" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="41" spans="1:7">
+      <c r="I40" t="s">
+        <v>473</v>
+      </c>
+      <c r="J40" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -3525,8 +3762,14 @@
       <c r="G41" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="42" spans="1:7">
+      <c r="I41" t="s">
+        <v>473</v>
+      </c>
+      <c r="J41" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -3548,8 +3791,14 @@
       <c r="G42" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="43" spans="1:7">
+      <c r="I42" t="s">
+        <v>473</v>
+      </c>
+      <c r="J42" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -3571,8 +3820,14 @@
       <c r="G43" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="44" spans="1:7">
+      <c r="I43" t="s">
+        <v>473</v>
+      </c>
+      <c r="J43" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -3594,8 +3849,14 @@
       <c r="G44" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="45" spans="1:7">
+      <c r="I44" t="s">
+        <v>473</v>
+      </c>
+      <c r="J44" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -3617,8 +3878,14 @@
       <c r="G45" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="46" spans="1:7">
+      <c r="I45" t="s">
+        <v>473</v>
+      </c>
+      <c r="J45" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -3640,8 +3907,14 @@
       <c r="G46" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="47" spans="1:7">
+      <c r="I46" t="s">
+        <v>473</v>
+      </c>
+      <c r="J46" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -3663,8 +3936,14 @@
       <c r="G47" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="48" spans="1:7">
+      <c r="I47" t="s">
+        <v>473</v>
+      </c>
+      <c r="J47" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -3686,8 +3965,14 @@
       <c r="G48" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="49" spans="1:7">
+      <c r="I48" t="s">
+        <v>473</v>
+      </c>
+      <c r="J48" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -3709,8 +3994,14 @@
       <c r="G49" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="50" spans="1:7">
+      <c r="I49" t="s">
+        <v>473</v>
+      </c>
+      <c r="J49" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -3732,8 +4023,14 @@
       <c r="G50" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="51" spans="1:7">
+      <c r="I50" t="s">
+        <v>473</v>
+      </c>
+      <c r="J50" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -3755,8 +4052,14 @@
       <c r="G51" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="52" spans="1:7">
+      <c r="I51" t="s">
+        <v>473</v>
+      </c>
+      <c r="J51" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -3778,8 +4081,14 @@
       <c r="G52" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="53" spans="1:7">
+      <c r="I52" t="s">
+        <v>473</v>
+      </c>
+      <c r="J52" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
       <c r="A53" t="s">
         <v>51</v>
       </c>
@@ -3801,8 +4110,14 @@
       <c r="G53" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="54" spans="1:7">
+      <c r="I53" t="s">
+        <v>473</v>
+      </c>
+      <c r="J53" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -3824,8 +4139,14 @@
       <c r="G54" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="55" spans="1:7">
+      <c r="I54" t="s">
+        <v>473</v>
+      </c>
+      <c r="J54" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -3847,8 +4168,14 @@
       <c r="G55" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="56" spans="1:7">
+      <c r="I55" t="s">
+        <v>473</v>
+      </c>
+      <c r="J55" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
       <c r="A56" t="s">
         <v>54</v>
       </c>
@@ -3870,8 +4197,14 @@
       <c r="G56" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="57" spans="1:7">
+      <c r="I56" t="s">
+        <v>473</v>
+      </c>
+      <c r="J56" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -3893,8 +4226,14 @@
       <c r="G57" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="58" spans="1:7">
+      <c r="I57" t="s">
+        <v>473</v>
+      </c>
+      <c r="J57" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
       <c r="A58" t="s">
         <v>56</v>
       </c>
@@ -3916,8 +4255,14 @@
       <c r="G58" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="59" spans="1:7">
+      <c r="I58" t="s">
+        <v>473</v>
+      </c>
+      <c r="J58" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
       <c r="A59" t="s">
         <v>57</v>
       </c>
@@ -3939,8 +4284,14 @@
       <c r="G59" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="60" spans="1:7">
+      <c r="I59" t="s">
+        <v>473</v>
+      </c>
+      <c r="J59" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
       <c r="A60" t="s">
         <v>58</v>
       </c>
@@ -3962,8 +4313,14 @@
       <c r="G60" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="61" spans="1:7">
+      <c r="I60" t="s">
+        <v>473</v>
+      </c>
+      <c r="J60" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
       <c r="A61" t="s">
         <v>59</v>
       </c>
@@ -3985,8 +4342,14 @@
       <c r="G61" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="62" spans="1:7">
+      <c r="I61" t="s">
+        <v>473</v>
+      </c>
+      <c r="J61" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
       <c r="A62" t="s">
         <v>60</v>
       </c>
@@ -4008,8 +4371,14 @@
       <c r="G62" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="63" spans="1:7">
+      <c r="I62" t="s">
+        <v>473</v>
+      </c>
+      <c r="J62" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
       <c r="A63" t="s">
         <v>61</v>
       </c>
@@ -4031,8 +4400,14 @@
       <c r="G63" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="64" spans="1:7">
+      <c r="I63" t="s">
+        <v>473</v>
+      </c>
+      <c r="J63" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
       <c r="A64" t="s">
         <v>62</v>
       </c>
@@ -4054,8 +4429,14 @@
       <c r="G64" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="65" spans="1:7">
+      <c r="I64" t="s">
+        <v>473</v>
+      </c>
+      <c r="J64" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
       <c r="A65" t="s">
         <v>63</v>
       </c>
@@ -4077,8 +4458,14 @@
       <c r="G65" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="66" spans="1:7">
+      <c r="I65" t="s">
+        <v>473</v>
+      </c>
+      <c r="J65" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10">
       <c r="A66" t="s">
         <v>64</v>
       </c>
@@ -4100,8 +4487,14 @@
       <c r="G66" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="67" spans="1:7">
+      <c r="I66" t="s">
+        <v>473</v>
+      </c>
+      <c r="J66" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10">
       <c r="A67" t="s">
         <v>65</v>
       </c>
@@ -4123,8 +4516,14 @@
       <c r="G67" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="68" spans="1:7">
+      <c r="I67" t="s">
+        <v>473</v>
+      </c>
+      <c r="J67" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10">
       <c r="A68" t="s">
         <v>66</v>
       </c>
@@ -4146,8 +4545,14 @@
       <c r="G68" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="69" spans="1:7">
+      <c r="I68" t="s">
+        <v>473</v>
+      </c>
+      <c r="J68" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10">
       <c r="A69" t="s">
         <v>67</v>
       </c>
@@ -4169,8 +4574,14 @@
       <c r="G69" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="70" spans="1:7">
+      <c r="I69" t="s">
+        <v>473</v>
+      </c>
+      <c r="J69" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10">
       <c r="A70" t="s">
         <v>68</v>
       </c>
@@ -4192,8 +4603,14 @@
       <c r="G70" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="71" spans="1:7">
+      <c r="I70" t="s">
+        <v>473</v>
+      </c>
+      <c r="J70" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10">
       <c r="A71" t="s">
         <v>69</v>
       </c>
@@ -4215,8 +4632,14 @@
       <c r="G71" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="72" spans="1:7">
+      <c r="I71" t="s">
+        <v>473</v>
+      </c>
+      <c r="J71" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10">
       <c r="A72" t="s">
         <v>70</v>
       </c>
@@ -4238,8 +4661,14 @@
       <c r="G72" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="73" spans="1:7">
+      <c r="I72" t="s">
+        <v>473</v>
+      </c>
+      <c r="J72" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10">
       <c r="A73" t="s">
         <v>71</v>
       </c>
@@ -4261,8 +4690,14 @@
       <c r="G73" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="74" spans="1:7">
+      <c r="I73" t="s">
+        <v>473</v>
+      </c>
+      <c r="J73" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10">
       <c r="A74" t="s">
         <v>72</v>
       </c>
@@ -4284,8 +4719,14 @@
       <c r="G74" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="75" spans="1:7">
+      <c r="I74" t="s">
+        <v>473</v>
+      </c>
+      <c r="J74" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10">
       <c r="A75" t="s">
         <v>73</v>
       </c>
@@ -4307,8 +4748,14 @@
       <c r="G75" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="76" spans="1:7">
+      <c r="I75" t="s">
+        <v>473</v>
+      </c>
+      <c r="J75" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10">
       <c r="A76" t="s">
         <v>74</v>
       </c>
@@ -4330,8 +4777,14 @@
       <c r="G76" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="77" spans="1:7">
+      <c r="I76" t="s">
+        <v>473</v>
+      </c>
+      <c r="J76" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10">
       <c r="A77" t="s">
         <v>75</v>
       </c>
@@ -4353,8 +4806,14 @@
       <c r="G77" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="78" spans="1:7">
+      <c r="I77" t="s">
+        <v>473</v>
+      </c>
+      <c r="J77" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10">
       <c r="A78" t="s">
         <v>76</v>
       </c>
@@ -4376,8 +4835,14 @@
       <c r="G78" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="79" spans="1:7">
+      <c r="I78" t="s">
+        <v>473</v>
+      </c>
+      <c r="J78" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10">
       <c r="A79" t="s">
         <v>77</v>
       </c>
@@ -4399,8 +4864,14 @@
       <c r="G79" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="80" spans="1:7">
+      <c r="I79" t="s">
+        <v>473</v>
+      </c>
+      <c r="J79" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10">
       <c r="A80" t="s">
         <v>78</v>
       </c>
@@ -4422,8 +4893,14 @@
       <c r="G80" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="81" spans="1:7">
+      <c r="I80" t="s">
+        <v>473</v>
+      </c>
+      <c r="J80" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10">
       <c r="A81" t="s">
         <v>79</v>
       </c>
@@ -4445,8 +4922,14 @@
       <c r="G81" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="82" spans="1:7">
+      <c r="I81" t="s">
+        <v>473</v>
+      </c>
+      <c r="J81" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10">
       <c r="A82" t="s">
         <v>80</v>
       </c>
@@ -4468,8 +4951,14 @@
       <c r="G82" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="83" spans="1:7">
+      <c r="I82" t="s">
+        <v>473</v>
+      </c>
+      <c r="J82" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10">
       <c r="A83" t="s">
         <v>81</v>
       </c>
@@ -4491,8 +4980,14 @@
       <c r="G83" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="84" spans="1:7">
+      <c r="I83" t="s">
+        <v>473</v>
+      </c>
+      <c r="J83" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10">
       <c r="A84" t="s">
         <v>82</v>
       </c>
@@ -4514,8 +5009,14 @@
       <c r="G84" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="85" spans="1:7">
+      <c r="I84" t="s">
+        <v>473</v>
+      </c>
+      <c r="J84" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10">
       <c r="A85" t="s">
         <v>83</v>
       </c>
@@ -4537,8 +5038,14 @@
       <c r="G85" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="86" spans="1:7">
+      <c r="I85" t="s">
+        <v>473</v>
+      </c>
+      <c r="J85" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10">
       <c r="A86" t="s">
         <v>84</v>
       </c>
@@ -4560,8 +5067,14 @@
       <c r="G86" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="87" spans="1:7">
+      <c r="I86" t="s">
+        <v>473</v>
+      </c>
+      <c r="J86" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10">
       <c r="A87" t="s">
         <v>85</v>
       </c>
@@ -4583,8 +5096,14 @@
       <c r="G87" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="88" spans="1:7">
+      <c r="I87" t="s">
+        <v>473</v>
+      </c>
+      <c r="J87" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10">
       <c r="A88" t="s">
         <v>86</v>
       </c>
@@ -4606,8 +5125,14 @@
       <c r="G88" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="89" spans="1:7">
+      <c r="I88" t="s">
+        <v>473</v>
+      </c>
+      <c r="J88" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10">
       <c r="A89" t="s">
         <v>87</v>
       </c>
@@ -4629,8 +5154,14 @@
       <c r="G89" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="90" spans="1:7">
+      <c r="I89" t="s">
+        <v>473</v>
+      </c>
+      <c r="J89" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10">
       <c r="A90" t="s">
         <v>88</v>
       </c>
@@ -4652,8 +5183,14 @@
       <c r="G90" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="91" spans="1:7">
+      <c r="I90" t="s">
+        <v>473</v>
+      </c>
+      <c r="J90" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10">
       <c r="A91" t="s">
         <v>89</v>
       </c>
@@ -4675,8 +5212,14 @@
       <c r="G91" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="92" spans="1:7">
+      <c r="I91" t="s">
+        <v>473</v>
+      </c>
+      <c r="J91" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10">
       <c r="A92" t="s">
         <v>90</v>
       </c>
@@ -4698,8 +5241,14 @@
       <c r="G92" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="93" spans="1:7">
+      <c r="I92" t="s">
+        <v>473</v>
+      </c>
+      <c r="J92" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10">
       <c r="A93" t="s">
         <v>91</v>
       </c>
@@ -4721,8 +5270,14 @@
       <c r="G93" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="94" spans="1:7">
+      <c r="I93" t="s">
+        <v>473</v>
+      </c>
+      <c r="J93" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10">
       <c r="A94" t="s">
         <v>92</v>
       </c>
@@ -4744,8 +5299,14 @@
       <c r="G94" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="95" spans="1:7">
+      <c r="I94" t="s">
+        <v>473</v>
+      </c>
+      <c r="J94" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10">
       <c r="A95" t="s">
         <v>93</v>
       </c>
@@ -4767,8 +5328,14 @@
       <c r="G95" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="96" spans="1:7">
+      <c r="I95" t="s">
+        <v>473</v>
+      </c>
+      <c r="J95" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10">
       <c r="A96" t="s">
         <v>94</v>
       </c>
@@ -4790,8 +5357,14 @@
       <c r="G96" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="97" spans="1:7">
+      <c r="I96" t="s">
+        <v>473</v>
+      </c>
+      <c r="J96" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10">
       <c r="A97" t="s">
         <v>95</v>
       </c>
@@ -4813,8 +5386,14 @@
       <c r="G97" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="98" spans="1:7">
+      <c r="I97" t="s">
+        <v>473</v>
+      </c>
+      <c r="J97" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10">
       <c r="A98" t="s">
         <v>96</v>
       </c>
@@ -4836,8 +5415,14 @@
       <c r="G98" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="99" spans="1:7">
+      <c r="I98" t="s">
+        <v>473</v>
+      </c>
+      <c r="J98" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10">
       <c r="A99" t="s">
         <v>97</v>
       </c>
@@ -4859,8 +5444,14 @@
       <c r="G99" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="100" spans="1:7">
+      <c r="I99" t="s">
+        <v>473</v>
+      </c>
+      <c r="J99" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10">
       <c r="A100" t="s">
         <v>98</v>
       </c>
@@ -4882,8 +5473,14 @@
       <c r="G100" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="101" spans="1:7">
+      <c r="I100" t="s">
+        <v>473</v>
+      </c>
+      <c r="J100" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10">
       <c r="A101" t="s">
         <v>99</v>
       </c>
@@ -4905,8 +5502,14 @@
       <c r="G101" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="102" spans="1:7">
+      <c r="I101" t="s">
+        <v>473</v>
+      </c>
+      <c r="J101" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10">
       <c r="A102" t="s">
         <v>100</v>
       </c>
@@ -4928,8 +5531,14 @@
       <c r="G102" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="103" spans="1:7">
+      <c r="I102" t="s">
+        <v>473</v>
+      </c>
+      <c r="J102" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10">
       <c r="A103" t="s">
         <v>101</v>
       </c>
@@ -4951,8 +5560,14 @@
       <c r="G103" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="104" spans="1:7">
+      <c r="I103" t="s">
+        <v>473</v>
+      </c>
+      <c r="J103" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10">
       <c r="A104" t="s">
         <v>102</v>
       </c>
@@ -4974,8 +5589,14 @@
       <c r="G104" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="105" spans="1:7">
+      <c r="I104" t="s">
+        <v>473</v>
+      </c>
+      <c r="J104" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10">
       <c r="A105" t="s">
         <v>103</v>
       </c>
@@ -4997,8 +5618,14 @@
       <c r="G105" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="106" spans="1:7">
+      <c r="I105" t="s">
+        <v>473</v>
+      </c>
+      <c r="J105" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10">
       <c r="A106" t="s">
         <v>104</v>
       </c>
@@ -5020,8 +5647,14 @@
       <c r="G106" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="107" spans="1:7">
+      <c r="I106" t="s">
+        <v>473</v>
+      </c>
+      <c r="J106" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10">
       <c r="A107" t="s">
         <v>105</v>
       </c>
@@ -5043,8 +5676,14 @@
       <c r="G107" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="108" spans="1:7">
+      <c r="I107" t="s">
+        <v>473</v>
+      </c>
+      <c r="J107" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10">
       <c r="A108" t="s">
         <v>106</v>
       </c>
@@ -5066,8 +5705,14 @@
       <c r="G108" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="109" spans="1:7">
+      <c r="I108" t="s">
+        <v>473</v>
+      </c>
+      <c r="J108" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10">
       <c r="A109" t="s">
         <v>107</v>
       </c>
@@ -5089,8 +5734,14 @@
       <c r="G109" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="110" spans="1:7">
+      <c r="I109" t="s">
+        <v>473</v>
+      </c>
+      <c r="J109" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10">
       <c r="A110" t="s">
         <v>108</v>
       </c>
@@ -5112,8 +5763,14 @@
       <c r="G110" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="111" spans="1:7">
+      <c r="I110" t="s">
+        <v>473</v>
+      </c>
+      <c r="J110" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10">
       <c r="A111" t="s">
         <v>109</v>
       </c>
@@ -5135,8 +5792,14 @@
       <c r="G111" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="112" spans="1:7">
+      <c r="I111" t="s">
+        <v>473</v>
+      </c>
+      <c r="J111" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10">
       <c r="A112" t="s">
         <v>110</v>
       </c>
@@ -5158,8 +5821,14 @@
       <c r="G112" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="113" spans="1:7">
+      <c r="I112" t="s">
+        <v>473</v>
+      </c>
+      <c r="J112" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10">
       <c r="A113" t="s">
         <v>111</v>
       </c>
@@ -5181,8 +5850,14 @@
       <c r="G113" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="114" spans="1:7">
+      <c r="I113" t="s">
+        <v>473</v>
+      </c>
+      <c r="J113" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10">
       <c r="A114" t="s">
         <v>112</v>
       </c>
@@ -5204,8 +5879,14 @@
       <c r="G114" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="115" spans="1:7">
+      <c r="I114" t="s">
+        <v>473</v>
+      </c>
+      <c r="J114" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10">
       <c r="A115" t="s">
         <v>113</v>
       </c>
@@ -5227,8 +5908,14 @@
       <c r="G115" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="116" spans="1:7">
+      <c r="I115" t="s">
+        <v>473</v>
+      </c>
+      <c r="J115" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10">
       <c r="A116" t="s">
         <v>114</v>
       </c>
@@ -5250,8 +5937,14 @@
       <c r="G116" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="117" spans="1:7">
+      <c r="I116" t="s">
+        <v>473</v>
+      </c>
+      <c r="J116" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10">
       <c r="A117" t="s">
         <v>115</v>
       </c>
@@ -5273,8 +5966,14 @@
       <c r="G117" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="118" spans="1:7">
+      <c r="I117" t="s">
+        <v>473</v>
+      </c>
+      <c r="J117" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10">
       <c r="A118" t="s">
         <v>116</v>
       </c>
@@ -5296,8 +5995,14 @@
       <c r="G118" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="119" spans="1:7">
+      <c r="I118" t="s">
+        <v>473</v>
+      </c>
+      <c r="J118" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10">
       <c r="A119" t="s">
         <v>117</v>
       </c>
@@ -5319,8 +6024,14 @@
       <c r="G119" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="120" spans="1:7">
+      <c r="I119" t="s">
+        <v>473</v>
+      </c>
+      <c r="J119" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10">
       <c r="A120" t="s">
         <v>118</v>
       </c>
@@ -5342,8 +6053,14 @@
       <c r="G120" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="121" spans="1:7">
+      <c r="I120" t="s">
+        <v>473</v>
+      </c>
+      <c r="J120" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10">
       <c r="A121" t="s">
         <v>119</v>
       </c>
@@ -5365,8 +6082,14 @@
       <c r="G121" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="122" spans="1:7">
+      <c r="I121" t="s">
+        <v>473</v>
+      </c>
+      <c r="J121" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10">
       <c r="A122" t="s">
         <v>120</v>
       </c>
@@ -5388,8 +6111,14 @@
       <c r="G122" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="123" spans="1:7">
+      <c r="I122" t="s">
+        <v>473</v>
+      </c>
+      <c r="J122" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10">
       <c r="A123" t="s">
         <v>121</v>
       </c>
@@ -5411,8 +6140,14 @@
       <c r="G123" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="124" spans="1:7">
+      <c r="I123" t="s">
+        <v>473</v>
+      </c>
+      <c r="J123" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10">
       <c r="A124" t="s">
         <v>122</v>
       </c>
@@ -5434,8 +6169,14 @@
       <c r="G124" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="125" spans="1:7">
+      <c r="I124" t="s">
+        <v>473</v>
+      </c>
+      <c r="J124" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10">
       <c r="A125" t="s">
         <v>123</v>
       </c>
@@ -5457,8 +6198,14 @@
       <c r="G125" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="126" spans="1:7">
+      <c r="I125" t="s">
+        <v>473</v>
+      </c>
+      <c r="J125" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10">
       <c r="A126" t="s">
         <v>124</v>
       </c>
@@ -5480,8 +6227,14 @@
       <c r="G126" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="127" spans="1:7">
+      <c r="I126" t="s">
+        <v>473</v>
+      </c>
+      <c r="J126" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10">
       <c r="A127" t="s">
         <v>125</v>
       </c>
@@ -5503,8 +6256,14 @@
       <c r="G127" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="128" spans="1:7">
+      <c r="I127" t="s">
+        <v>473</v>
+      </c>
+      <c r="J127" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10">
       <c r="A128" t="s">
         <v>126</v>
       </c>
@@ -5526,8 +6285,14 @@
       <c r="G128" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="129" spans="1:7">
+      <c r="I128" t="s">
+        <v>473</v>
+      </c>
+      <c r="J128" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10">
       <c r="A129" t="s">
         <v>127</v>
       </c>
@@ -5549,8 +6314,14 @@
       <c r="G129" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="130" spans="1:7">
+      <c r="I129" t="s">
+        <v>473</v>
+      </c>
+      <c r="J129" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10">
       <c r="A130" t="s">
         <v>128</v>
       </c>
@@ -5572,8 +6343,14 @@
       <c r="G130" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="131" spans="1:7">
+      <c r="I130" t="s">
+        <v>473</v>
+      </c>
+      <c r="J130" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10">
       <c r="A131" t="s">
         <v>129</v>
       </c>
@@ -5595,8 +6372,14 @@
       <c r="G131" s="2" t="s">
         <v>473</v>
       </c>
-    </row>
-    <row r="132" spans="1:7">
+      <c r="I131" t="s">
+        <v>473</v>
+      </c>
+      <c r="J131" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10">
       <c r="A132" t="s">
         <v>130</v>
       </c>
@@ -5618,8 +6401,14 @@
       <c r="G132" s="2" t="s">
         <v>473</v>
       </c>
-    </row>
-    <row r="133" spans="1:7">
+      <c r="I132" t="s">
+        <v>473</v>
+      </c>
+      <c r="J132" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10">
       <c r="A133" t="s">
         <v>131</v>
       </c>
@@ -5641,8 +6430,14 @@
       <c r="G133" s="2" t="s">
         <v>473</v>
       </c>
-    </row>
-    <row r="134" spans="1:7">
+      <c r="I133" t="s">
+        <v>473</v>
+      </c>
+      <c r="J133" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10">
       <c r="A134" t="s">
         <v>132</v>
       </c>
@@ -5664,8 +6459,14 @@
       <c r="G134" s="2" t="s">
         <v>473</v>
       </c>
-    </row>
-    <row r="135" spans="1:7">
+      <c r="I134" t="s">
+        <v>473</v>
+      </c>
+      <c r="J134" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10">
       <c r="A135" t="s">
         <v>133</v>
       </c>
@@ -5685,6 +6486,12 @@
         <v>473</v>
       </c>
       <c r="G135" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="I135" t="s">
+        <v>473</v>
+      </c>
+      <c r="J135" t="s">
         <v>473</v>
       </c>
     </row>
@@ -5698,7 +6505,7 @@
   <dimension ref="A1:J58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="I2" sqref="I2:J58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5767,6 +6574,12 @@
       <c r="G2" s="2" t="s">
         <v>476</v>
       </c>
+      <c r="I2" t="s">
+        <v>473</v>
+      </c>
+      <c r="J2" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
@@ -5790,6 +6603,12 @@
       <c r="G3" s="2" t="s">
         <v>478</v>
       </c>
+      <c r="I3" t="s">
+        <v>473</v>
+      </c>
+      <c r="J3" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
@@ -5813,6 +6632,12 @@
       <c r="G4" s="2" t="s">
         <v>478</v>
       </c>
+      <c r="I4" t="s">
+        <v>473</v>
+      </c>
+      <c r="J4" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
@@ -5836,6 +6661,12 @@
       <c r="G5" s="2" t="s">
         <v>476</v>
       </c>
+      <c r="I5" t="s">
+        <v>473</v>
+      </c>
+      <c r="J5" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
@@ -5859,6 +6690,12 @@
       <c r="G6" s="2" t="s">
         <v>478</v>
       </c>
+      <c r="I6" t="s">
+        <v>473</v>
+      </c>
+      <c r="J6" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
@@ -5882,6 +6719,12 @@
       <c r="G7" s="2" t="s">
         <v>478</v>
       </c>
+      <c r="I7" t="s">
+        <v>473</v>
+      </c>
+      <c r="J7" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
@@ -5905,6 +6748,12 @@
       <c r="G8" s="2" t="s">
         <v>476</v>
       </c>
+      <c r="I8" t="s">
+        <v>473</v>
+      </c>
+      <c r="J8" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
@@ -5928,6 +6777,12 @@
       <c r="G9" s="2" t="s">
         <v>478</v>
       </c>
+      <c r="I9" t="s">
+        <v>473</v>
+      </c>
+      <c r="J9" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
@@ -5951,6 +6806,12 @@
       <c r="G10" s="2" t="s">
         <v>478</v>
       </c>
+      <c r="I10" t="s">
+        <v>473</v>
+      </c>
+      <c r="J10" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
@@ -5974,6 +6835,12 @@
       <c r="G11" s="2" t="s">
         <v>478</v>
       </c>
+      <c r="I11" t="s">
+        <v>473</v>
+      </c>
+      <c r="J11" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
@@ -5997,6 +6864,12 @@
       <c r="G12" s="2" t="s">
         <v>478</v>
       </c>
+      <c r="I12" t="s">
+        <v>473</v>
+      </c>
+      <c r="J12" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
@@ -6020,6 +6893,12 @@
       <c r="G13" s="2" t="s">
         <v>478</v>
       </c>
+      <c r="I13" t="s">
+        <v>473</v>
+      </c>
+      <c r="J13" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
@@ -6043,6 +6922,12 @@
       <c r="G14" s="2" t="s">
         <v>476</v>
       </c>
+      <c r="I14" t="s">
+        <v>473</v>
+      </c>
+      <c r="J14" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
@@ -6066,6 +6951,12 @@
       <c r="G15" s="2" t="s">
         <v>478</v>
       </c>
+      <c r="I15" t="s">
+        <v>473</v>
+      </c>
+      <c r="J15" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
@@ -6089,8 +6980,14 @@
       <c r="G16" s="2" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="I16" t="s">
+        <v>473</v>
+      </c>
+      <c r="J16" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>149</v>
       </c>
@@ -6112,8 +7009,14 @@
       <c r="G17" s="2" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="I17" t="s">
+        <v>473</v>
+      </c>
+      <c r="J17" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
         <v>150</v>
       </c>
@@ -6135,8 +7038,14 @@
       <c r="G18" s="2" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="I18" t="s">
+        <v>473</v>
+      </c>
+      <c r="J18" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
         <v>151</v>
       </c>
@@ -6158,8 +7067,14 @@
       <c r="G19" s="2" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="20" spans="1:7">
+      <c r="I19" t="s">
+        <v>473</v>
+      </c>
+      <c r="J19" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
         <v>152</v>
       </c>
@@ -6181,8 +7096,14 @@
       <c r="G20" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="I20" t="s">
+        <v>473</v>
+      </c>
+      <c r="J20" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
         <v>153</v>
       </c>
@@ -6204,8 +7125,14 @@
       <c r="G21" s="2" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="22" spans="1:7">
+      <c r="I21" t="s">
+        <v>473</v>
+      </c>
+      <c r="J21" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
         <v>154</v>
       </c>
@@ -6227,8 +7154,14 @@
       <c r="G22" s="2" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="23" spans="1:7">
+      <c r="I22" t="s">
+        <v>473</v>
+      </c>
+      <c r="J22" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" t="s">
         <v>155</v>
       </c>
@@ -6250,8 +7183,14 @@
       <c r="G23" s="2" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="24" spans="1:7">
+      <c r="I23" t="s">
+        <v>473</v>
+      </c>
+      <c r="J23" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" t="s">
         <v>156</v>
       </c>
@@ -6273,8 +7212,14 @@
       <c r="G24" s="2" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="25" spans="1:7">
+      <c r="I24" t="s">
+        <v>473</v>
+      </c>
+      <c r="J24" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" t="s">
         <v>157</v>
       </c>
@@ -6296,8 +7241,14 @@
       <c r="G25" s="2" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="26" spans="1:7">
+      <c r="I25" t="s">
+        <v>473</v>
+      </c>
+      <c r="J25" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" t="s">
         <v>158</v>
       </c>
@@ -6319,8 +7270,14 @@
       <c r="G26" s="2" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="27" spans="1:7">
+      <c r="I26" t="s">
+        <v>473</v>
+      </c>
+      <c r="J26" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" t="s">
         <v>159</v>
       </c>
@@ -6342,8 +7299,14 @@
       <c r="G27" s="2" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="28" spans="1:7">
+      <c r="I27" t="s">
+        <v>473</v>
+      </c>
+      <c r="J27" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" t="s">
         <v>160</v>
       </c>
@@ -6365,8 +7328,14 @@
       <c r="G28" s="2" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="29" spans="1:7">
+      <c r="I28" t="s">
+        <v>473</v>
+      </c>
+      <c r="J28" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29" t="s">
         <v>161</v>
       </c>
@@ -6388,8 +7357,14 @@
       <c r="G29" s="2" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="30" spans="1:7">
+      <c r="I29" t="s">
+        <v>473</v>
+      </c>
+      <c r="J29" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30" t="s">
         <v>162</v>
       </c>
@@ -6411,8 +7386,14 @@
       <c r="G30" s="2" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="31" spans="1:7">
+      <c r="I30" t="s">
+        <v>473</v>
+      </c>
+      <c r="J30" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31" t="s">
         <v>163</v>
       </c>
@@ -6434,8 +7415,14 @@
       <c r="G31" s="2" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="32" spans="1:7">
+      <c r="I31" t="s">
+        <v>473</v>
+      </c>
+      <c r="J31" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32" t="s">
         <v>164</v>
       </c>
@@ -6457,8 +7444,14 @@
       <c r="G32" s="2" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="33" spans="1:7">
+      <c r="I32" t="s">
+        <v>473</v>
+      </c>
+      <c r="J32" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33" t="s">
         <v>165</v>
       </c>
@@ -6480,8 +7473,14 @@
       <c r="G33" s="2" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="34" spans="1:7">
+      <c r="I33" t="s">
+        <v>473</v>
+      </c>
+      <c r="J33" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34" t="s">
         <v>166</v>
       </c>
@@ -6503,8 +7502,14 @@
       <c r="G34" s="2" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="35" spans="1:7">
+      <c r="I34" t="s">
+        <v>473</v>
+      </c>
+      <c r="J34" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35" t="s">
         <v>167</v>
       </c>
@@ -6526,8 +7531,14 @@
       <c r="G35" s="2" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="36" spans="1:7">
+      <c r="I35" t="s">
+        <v>473</v>
+      </c>
+      <c r="J35" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36" t="s">
         <v>168</v>
       </c>
@@ -6549,8 +7560,14 @@
       <c r="G36" s="2" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="37" spans="1:7">
+      <c r="I36" t="s">
+        <v>473</v>
+      </c>
+      <c r="J36" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
       <c r="A37" t="s">
         <v>169</v>
       </c>
@@ -6572,8 +7589,14 @@
       <c r="G37" s="2" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="38" spans="1:7">
+      <c r="I37" t="s">
+        <v>473</v>
+      </c>
+      <c r="J37" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
       <c r="A38" t="s">
         <v>170</v>
       </c>
@@ -6595,8 +7618,14 @@
       <c r="G38" s="2" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="39" spans="1:7">
+      <c r="I38" t="s">
+        <v>473</v>
+      </c>
+      <c r="J38" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
       <c r="A39" t="s">
         <v>171</v>
       </c>
@@ -6618,8 +7647,14 @@
       <c r="G39" s="2" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="40" spans="1:7">
+      <c r="I39" t="s">
+        <v>473</v>
+      </c>
+      <c r="J39" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
       <c r="A40" t="s">
         <v>172</v>
       </c>
@@ -6641,8 +7676,14 @@
       <c r="G40" s="2" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="41" spans="1:7">
+      <c r="I40" t="s">
+        <v>473</v>
+      </c>
+      <c r="J40" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
       <c r="A41" t="s">
         <v>173</v>
       </c>
@@ -6664,8 +7705,14 @@
       <c r="G41" s="2" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="42" spans="1:7">
+      <c r="I41" t="s">
+        <v>473</v>
+      </c>
+      <c r="J41" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
       <c r="A42" t="s">
         <v>174</v>
       </c>
@@ -6687,8 +7734,14 @@
       <c r="G42" s="2" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="43" spans="1:7">
+      <c r="I42" t="s">
+        <v>473</v>
+      </c>
+      <c r="J42" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
       <c r="A43" t="s">
         <v>175</v>
       </c>
@@ -6710,8 +7763,14 @@
       <c r="G43" s="2" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="44" spans="1:7">
+      <c r="I43" t="s">
+        <v>473</v>
+      </c>
+      <c r="J43" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
       <c r="A44" t="s">
         <v>176</v>
       </c>
@@ -6733,8 +7792,14 @@
       <c r="G44" s="2" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="45" spans="1:7">
+      <c r="I44" t="s">
+        <v>473</v>
+      </c>
+      <c r="J44" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
       <c r="A45" t="s">
         <v>177</v>
       </c>
@@ -6756,8 +7821,14 @@
       <c r="G45" s="2" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="46" spans="1:7">
+      <c r="I45" t="s">
+        <v>473</v>
+      </c>
+      <c r="J45" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
       <c r="A46" t="s">
         <v>178</v>
       </c>
@@ -6779,8 +7850,14 @@
       <c r="G46" s="2" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="47" spans="1:7">
+      <c r="I46" t="s">
+        <v>473</v>
+      </c>
+      <c r="J46" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
       <c r="A47" t="s">
         <v>179</v>
       </c>
@@ -6802,8 +7879,14 @@
       <c r="G47" s="2" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="48" spans="1:7">
+      <c r="I47" t="s">
+        <v>473</v>
+      </c>
+      <c r="J47" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
       <c r="A48" t="s">
         <v>180</v>
       </c>
@@ -6825,8 +7908,14 @@
       <c r="G48" s="2" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="49" spans="1:7">
+      <c r="I48" t="s">
+        <v>473</v>
+      </c>
+      <c r="J48" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
       <c r="A49" t="s">
         <v>181</v>
       </c>
@@ -6848,8 +7937,14 @@
       <c r="G49" s="2" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="50" spans="1:7">
+      <c r="I49" t="s">
+        <v>473</v>
+      </c>
+      <c r="J49" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
       <c r="A50" t="s">
         <v>182</v>
       </c>
@@ -6871,8 +7966,14 @@
       <c r="G50" s="2" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="51" spans="1:7">
+      <c r="I50" t="s">
+        <v>473</v>
+      </c>
+      <c r="J50" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
       <c r="A51" t="s">
         <v>183</v>
       </c>
@@ -6894,8 +7995,14 @@
       <c r="G51" s="2" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="52" spans="1:7">
+      <c r="I51" t="s">
+        <v>473</v>
+      </c>
+      <c r="J51" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
       <c r="A52" t="s">
         <v>184</v>
       </c>
@@ -6917,8 +8024,14 @@
       <c r="G52" s="2" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="53" spans="1:7">
+      <c r="I52" t="s">
+        <v>473</v>
+      </c>
+      <c r="J52" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
       <c r="A53" t="s">
         <v>185</v>
       </c>
@@ -6940,8 +8053,14 @@
       <c r="G53" s="2" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="54" spans="1:7">
+      <c r="I53" t="s">
+        <v>473</v>
+      </c>
+      <c r="J53" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
       <c r="A54" t="s">
         <v>186</v>
       </c>
@@ -6963,8 +8082,14 @@
       <c r="G54" s="2" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="55" spans="1:7">
+      <c r="I54" t="s">
+        <v>473</v>
+      </c>
+      <c r="J54" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
       <c r="A55" t="s">
         <v>187</v>
       </c>
@@ -6986,8 +8111,14 @@
       <c r="G55" s="2" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="56" spans="1:7">
+      <c r="I55" t="s">
+        <v>473</v>
+      </c>
+      <c r="J55" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
       <c r="A56" t="s">
         <v>188</v>
       </c>
@@ -7009,8 +8140,14 @@
       <c r="G56" s="2" t="s">
         <v>473</v>
       </c>
-    </row>
-    <row r="57" spans="1:7">
+      <c r="I56" t="s">
+        <v>473</v>
+      </c>
+      <c r="J56" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
       <c r="A57" t="s">
         <v>189</v>
       </c>
@@ -7032,8 +8169,14 @@
       <c r="G57" s="2" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="58" spans="1:7">
+      <c r="I57" t="s">
+        <v>473</v>
+      </c>
+      <c r="J57" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
       <c r="A58" t="s">
         <v>190</v>
       </c>
@@ -7054,6 +8197,12 @@
       </c>
       <c r="G58" s="2" t="s">
         <v>481</v>
+      </c>
+      <c r="I58" t="s">
+        <v>473</v>
+      </c>
+      <c r="J58" t="s">
+        <v>473</v>
       </c>
     </row>
   </sheetData>
@@ -7065,22 +8214,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J105"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1:I1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H81" sqref="H81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="43.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="39.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="66.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1">
@@ -9426,13 +10576,13 @@
         <v>473</v>
       </c>
       <c r="G81" s="16" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="H81" s="16" t="s">
-        <v>473</v>
+        <v>609</v>
       </c>
       <c r="I81" s="16" t="s">
-        <v>473</v>
+        <v>608</v>
       </c>
     </row>
     <row r="82" spans="1:10">
@@ -9457,10 +10607,10 @@
       <c r="G82" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="H82" s="16" t="s">
-        <v>473</v>
-      </c>
-      <c r="I82" s="16" t="s">
+      <c r="H82" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="I82" s="2" t="s">
         <v>473</v>
       </c>
     </row>
@@ -10145,7 +11295,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10214,6 +11364,12 @@
       <c r="G2" s="2" t="s">
         <v>478</v>
       </c>
+      <c r="I2" t="s">
+        <v>473</v>
+      </c>
+      <c r="J2" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
@@ -10237,6 +11393,12 @@
       <c r="G3" s="2" t="s">
         <v>476</v>
       </c>
+      <c r="I3" t="s">
+        <v>473</v>
+      </c>
+      <c r="J3" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
@@ -10260,6 +11422,12 @@
       <c r="G4" s="2" t="s">
         <v>480</v>
       </c>
+      <c r="I4" t="s">
+        <v>473</v>
+      </c>
+      <c r="J4" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
@@ -10283,6 +11451,12 @@
       <c r="G5" s="3" t="s">
         <v>482</v>
       </c>
+      <c r="I5" t="s">
+        <v>473</v>
+      </c>
+      <c r="J5" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
@@ -10304,6 +11478,12 @@
         <v>473</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="I6" t="s">
+        <v>473</v>
+      </c>
+      <c r="J6" t="s">
         <v>473</v>
       </c>
     </row>
@@ -10316,8 +11496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J247"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A215" workbookViewId="0">
-      <selection activeCell="G238" sqref="G238"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10546,7 +11726,7 @@
         <v>473</v>
       </c>
       <c r="G7" t="s">
-        <v>608</v>
+        <v>481</v>
       </c>
       <c r="H7" t="s">
         <v>473</v>
@@ -10578,7 +11758,7 @@
         <v>473</v>
       </c>
       <c r="G8" t="s">
-        <v>608</v>
+        <v>481</v>
       </c>
       <c r="H8" t="s">
         <v>473</v>
@@ -10610,7 +11790,7 @@
         <v>473</v>
       </c>
       <c r="G9" t="s">
-        <v>608</v>
+        <v>481</v>
       </c>
       <c r="H9" t="s">
         <v>473</v>
@@ -10642,7 +11822,7 @@
         <v>473</v>
       </c>
       <c r="G10" t="s">
-        <v>608</v>
+        <v>481</v>
       </c>
       <c r="H10" t="s">
         <v>473</v>
@@ -10674,7 +11854,7 @@
         <v>473</v>
       </c>
       <c r="G11" t="s">
-        <v>608</v>
+        <v>481</v>
       </c>
       <c r="H11" t="s">
         <v>473</v>
@@ -10898,7 +12078,7 @@
         <v>473</v>
       </c>
       <c r="G18" t="s">
-        <v>608</v>
+        <v>481</v>
       </c>
       <c r="H18" t="s">
         <v>473</v>
@@ -10930,7 +12110,7 @@
         <v>473</v>
       </c>
       <c r="G19" t="s">
-        <v>608</v>
+        <v>481</v>
       </c>
       <c r="H19" t="s">
         <v>473</v>
@@ -10962,7 +12142,7 @@
         <v>473</v>
       </c>
       <c r="G20" t="s">
-        <v>608</v>
+        <v>481</v>
       </c>
       <c r="H20" t="s">
         <v>473</v>
@@ -10994,7 +12174,7 @@
         <v>473</v>
       </c>
       <c r="G21" t="s">
-        <v>608</v>
+        <v>481</v>
       </c>
       <c r="H21" t="s">
         <v>473</v>
@@ -11026,7 +12206,7 @@
         <v>473</v>
       </c>
       <c r="G22" t="s">
-        <v>608</v>
+        <v>481</v>
       </c>
       <c r="H22" t="s">
         <v>473</v>
@@ -11250,7 +12430,7 @@
         <v>473</v>
       </c>
       <c r="G29" t="s">
-        <v>608</v>
+        <v>481</v>
       </c>
       <c r="H29" t="s">
         <v>473</v>
@@ -11282,7 +12462,7 @@
         <v>473</v>
       </c>
       <c r="G30" t="s">
-        <v>608</v>
+        <v>481</v>
       </c>
       <c r="H30" t="s">
         <v>473</v>
@@ -11314,7 +12494,7 @@
         <v>473</v>
       </c>
       <c r="G31" t="s">
-        <v>608</v>
+        <v>481</v>
       </c>
       <c r="H31" t="s">
         <v>473</v>
@@ -11346,7 +12526,7 @@
         <v>473</v>
       </c>
       <c r="G32" t="s">
-        <v>608</v>
+        <v>481</v>
       </c>
       <c r="H32" t="s">
         <v>473</v>
@@ -11378,7 +12558,7 @@
         <v>473</v>
       </c>
       <c r="G33" t="s">
-        <v>608</v>
+        <v>481</v>
       </c>
       <c r="H33" t="s">
         <v>473</v>
@@ -11602,7 +12782,7 @@
         <v>473</v>
       </c>
       <c r="G40" t="s">
-        <v>608</v>
+        <v>481</v>
       </c>
       <c r="H40" t="s">
         <v>473</v>
@@ -11634,7 +12814,7 @@
         <v>473</v>
       </c>
       <c r="G41" t="s">
-        <v>608</v>
+        <v>481</v>
       </c>
       <c r="H41" t="s">
         <v>473</v>
@@ -11666,7 +12846,7 @@
         <v>473</v>
       </c>
       <c r="G42" t="s">
-        <v>608</v>
+        <v>481</v>
       </c>
       <c r="H42" t="s">
         <v>473</v>
@@ -11698,7 +12878,7 @@
         <v>473</v>
       </c>
       <c r="G43" t="s">
-        <v>608</v>
+        <v>481</v>
       </c>
       <c r="H43" t="s">
         <v>473</v>
@@ -11730,7 +12910,7 @@
         <v>473</v>
       </c>
       <c r="G44" t="s">
-        <v>608</v>
+        <v>481</v>
       </c>
       <c r="H44" t="s">
         <v>473</v>
@@ -12370,7 +13550,7 @@
         <v>473</v>
       </c>
       <c r="G64" t="s">
-        <v>608</v>
+        <v>481</v>
       </c>
       <c r="H64" t="s">
         <v>473</v>
@@ -12562,7 +13742,7 @@
         <v>473</v>
       </c>
       <c r="G70" t="s">
-        <v>608</v>
+        <v>481</v>
       </c>
       <c r="H70" t="s">
         <v>473</v>
@@ -12722,7 +13902,7 @@
         <v>473</v>
       </c>
       <c r="G75" t="s">
-        <v>608</v>
+        <v>481</v>
       </c>
       <c r="H75" t="s">
         <v>473</v>
@@ -12786,7 +13966,7 @@
         <v>473</v>
       </c>
       <c r="G77" t="s">
-        <v>608</v>
+        <v>481</v>
       </c>
       <c r="H77" t="s">
         <v>473</v>
@@ -12818,7 +13998,7 @@
         <v>473</v>
       </c>
       <c r="G78" t="s">
-        <v>608</v>
+        <v>481</v>
       </c>
       <c r="H78" t="s">
         <v>473</v>
@@ -12850,7 +14030,7 @@
         <v>473</v>
       </c>
       <c r="G79" t="s">
-        <v>608</v>
+        <v>481</v>
       </c>
       <c r="H79" t="s">
         <v>473</v>
@@ -12978,7 +14158,7 @@
         <v>473</v>
       </c>
       <c r="G83" t="s">
-        <v>608</v>
+        <v>481</v>
       </c>
       <c r="H83" t="s">
         <v>473</v>
@@ -13266,7 +14446,7 @@
         <v>473</v>
       </c>
       <c r="G92" t="s">
-        <v>608</v>
+        <v>481</v>
       </c>
       <c r="H92" t="s">
         <v>473</v>
@@ -13330,7 +14510,7 @@
         <v>473</v>
       </c>
       <c r="G94" t="s">
-        <v>608</v>
+        <v>481</v>
       </c>
       <c r="H94" t="s">
         <v>473</v>

</xml_diff>